<commit_message>
fixed bug with NaN in match
</commit_message>
<xml_diff>
--- a/upper-level_writing_sample_output.xlsx
+++ b/upper-level_writing_sample_output.xlsx
@@ -30,7 +30,7 @@
     <t>jane</t>
   </si>
   <si>
-    <t>derivational relations late</t>
+    <t>derivational relations middle</t>
   </si>
   <si>
     <t>spelled words</t>
@@ -708,6 +708,24 @@
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
       <c r="L4">
         <v>3</v>
       </c>
@@ -731,6 +749,24 @@
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
       <c r="L5">
         <v>3</v>
       </c>
@@ -748,7 +784,28 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
@@ -765,11 +822,32 @@
       <c r="B7" t="s">
         <v>50</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
         <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -785,6 +863,9 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
       <c r="D8">
         <v>1</v>
       </c>
@@ -793,6 +874,21 @@
       </c>
       <c r="F8">
         <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -811,8 +907,29 @@
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="F9">
         <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
       <c r="L9">
         <v>2</v>
@@ -828,11 +945,32 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -848,11 +986,32 @@
       <c r="B11" t="s">
         <v>25</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
         <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
       </c>
       <c r="L11">
         <v>2</v>
@@ -868,6 +1027,9 @@
       <c r="B12" t="s">
         <v>51</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
       <c r="D12">
         <v>1</v>
       </c>
@@ -875,6 +1037,21 @@
         <v>1</v>
       </c>
       <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
@@ -894,11 +1071,29 @@
       <c r="C13">
         <v>1</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
         <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -914,11 +1109,32 @@
       <c r="B14" t="s">
         <v>28</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
       <c r="G14">
         <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
       </c>
       <c r="L14">
         <v>2</v>
@@ -934,11 +1150,32 @@
       <c r="B15" t="s">
         <v>52</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
         <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -954,14 +1191,32 @@
       <c r="B16" t="s">
         <v>30</v>
       </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
         <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
       </c>
       <c r="L16">
         <v>3</v>
@@ -977,11 +1232,32 @@
       <c r="B17" t="s">
         <v>31</v>
       </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
         <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
       </c>
       <c r="L17">
         <v>2</v>
@@ -997,11 +1273,32 @@
       <c r="B18" t="s">
         <v>32</v>
       </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
         <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
       </c>
       <c r="L18">
         <v>2</v>
@@ -1017,11 +1314,32 @@
       <c r="B19" t="s">
         <v>33</v>
       </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
         <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
       </c>
       <c r="L19">
         <v>2</v>
@@ -1037,11 +1355,32 @@
       <c r="B20" t="s">
         <v>34</v>
       </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
       <c r="G20">
         <v>1</v>
       </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
       <c r="J20">
         <v>1</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
       </c>
       <c r="L20">
         <v>2</v>
@@ -1057,11 +1396,32 @@
       <c r="B21" t="s">
         <v>35</v>
       </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
       <c r="H21">
         <v>1</v>
       </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
       <c r="J21">
         <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
       </c>
       <c r="L21">
         <v>2</v>
@@ -1077,11 +1437,32 @@
       <c r="B22" t="s">
         <v>36</v>
       </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
       <c r="H22">
         <v>1</v>
       </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
       <c r="J22">
         <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
       </c>
       <c r="L22">
         <v>2</v>
@@ -1097,11 +1478,32 @@
       <c r="B23" t="s">
         <v>37</v>
       </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23">
         <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -1117,8 +1519,32 @@
       <c r="B24" t="s">
         <v>38</v>
       </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
       <c r="J24">
         <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -1135,16 +1561,19 @@
         <v>53</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1153,13 +1582,13 @@
         <v>1</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -1172,8 +1601,29 @@
       <c r="B26" t="s">
         <v>40</v>
       </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
       <c r="I26">
         <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -1192,8 +1642,29 @@
       <c r="B27" t="s">
         <v>41</v>
       </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
       <c r="G27">
         <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -1212,11 +1683,32 @@
       <c r="B28" t="s">
         <v>42</v>
       </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
         <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
       </c>
       <c r="L28">
         <v>2</v>
@@ -1232,7 +1724,28 @@
       <c r="B29" t="s">
         <v>54</v>
       </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
       <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
         <v>0</v>
       </c>
       <c r="K29">
@@ -1252,11 +1765,32 @@
       <c r="B30" t="s">
         <v>55</v>
       </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
       <c r="H30">
         <v>0</v>
       </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
       <c r="J30">
         <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
       </c>
       <c r="L30">
         <v>1</v>
@@ -1272,8 +1806,29 @@
       <c r="B31" t="s">
         <v>45</v>
       </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
       <c r="H31">
         <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -1292,11 +1847,32 @@
       <c r="B32" t="s">
         <v>56</v>
       </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
       <c r="G32">
         <v>0</v>
       </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
       <c r="J32">
         <v>1</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
       </c>
       <c r="L32">
         <v>1</v>
@@ -1312,11 +1888,29 @@
       <c r="B33" t="s">
         <v>57</v>
       </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33">
         <v>1</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -1335,8 +1929,29 @@
       <c r="B34" t="s">
         <v>48</v>
       </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
       <c r="H34">
         <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -1443,6 +2058,24 @@
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
       <c r="L4">
         <v>2</v>
       </c>
@@ -1466,6 +2099,24 @@
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
       <c r="L5">
         <v>3</v>
       </c>
@@ -1483,8 +2134,29 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="F6">
         <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -1500,11 +2172,32 @@
       <c r="B7" t="s">
         <v>21</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
         <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
       </c>
       <c r="L7">
         <v>2</v>
@@ -1520,6 +2213,9 @@
       <c r="B8" t="s">
         <v>60</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
       <c r="D8">
         <v>1</v>
       </c>
@@ -1527,6 +2223,21 @@
         <v>1</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
@@ -1546,7 +2257,28 @@
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
@@ -1563,11 +2295,32 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -1583,11 +2336,32 @@
       <c r="B11" t="s">
         <v>25</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
         <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
       </c>
       <c r="L11">
         <v>2</v>
@@ -1603,6 +2377,9 @@
       <c r="B12" t="s">
         <v>26</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
       <c r="D12">
         <v>1</v>
       </c>
@@ -1611,6 +2388,21 @@
       </c>
       <c r="F12">
         <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
       </c>
       <c r="L12">
         <v>3</v>
@@ -1629,11 +2421,29 @@
       <c r="C13">
         <v>1</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
         <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -1649,11 +2459,32 @@
       <c r="B14" t="s">
         <v>62</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
       <c r="D14">
         <v>0</v>
       </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
       <c r="G14">
         <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -1669,11 +2500,32 @@
       <c r="B15" t="s">
         <v>29</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
         <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
       </c>
       <c r="L15">
         <v>2</v>
@@ -1689,14 +2541,32 @@
       <c r="B16" t="s">
         <v>30</v>
       </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
         <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
       </c>
       <c r="L16">
         <v>3</v>
@@ -1712,11 +2582,32 @@
       <c r="B17" t="s">
         <v>63</v>
       </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
         <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -1732,11 +2623,32 @@
       <c r="B18" t="s">
         <v>32</v>
       </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
         <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
       </c>
       <c r="L18">
         <v>2</v>
@@ -1752,11 +2664,32 @@
       <c r="B19" t="s">
         <v>64</v>
       </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
         <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
       </c>
       <c r="L19">
         <v>2</v>
@@ -1772,11 +2705,32 @@
       <c r="B20" t="s">
         <v>34</v>
       </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
       <c r="G20">
         <v>1</v>
       </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
       <c r="J20">
         <v>1</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
       </c>
       <c r="L20">
         <v>2</v>
@@ -1792,11 +2746,32 @@
       <c r="B21" t="s">
         <v>65</v>
       </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
       <c r="H21">
         <v>0</v>
       </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
       <c r="J21">
         <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -1812,11 +2787,32 @@
       <c r="B22" t="s">
         <v>66</v>
       </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
       <c r="H22">
         <v>1</v>
       </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
       <c r="J22">
         <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
       </c>
       <c r="L22">
         <v>2</v>
@@ -1832,11 +2828,32 @@
       <c r="B23" t="s">
         <v>67</v>
       </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23">
         <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -1852,8 +2869,32 @@
       <c r="B24" t="s">
         <v>38</v>
       </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
       <c r="J24">
         <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -1870,16 +2911,19 @@
         <v>39</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1888,13 +2932,13 @@
         <v>1</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -1907,8 +2951,29 @@
       <c r="B26" t="s">
         <v>40</v>
       </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
       <c r="I26">
         <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -1927,8 +2992,29 @@
       <c r="B27" t="s">
         <v>68</v>
       </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
       <c r="G27">
         <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -1947,10 +3033,31 @@
       <c r="B28" t="s">
         <v>69</v>
       </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
@@ -1967,8 +3074,29 @@
       <c r="B29" t="s">
         <v>43</v>
       </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
       <c r="I29">
         <v>1</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -1987,11 +3115,32 @@
       <c r="B30" t="s">
         <v>44</v>
       </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
       <c r="H30">
         <v>1</v>
       </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
       <c r="J30">
         <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
       </c>
       <c r="L30">
         <v>2</v>
@@ -2007,7 +3156,28 @@
       <c r="B31" t="s">
         <v>70</v>
       </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
       <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
         <v>0</v>
       </c>
       <c r="K31">
@@ -2027,11 +3197,32 @@
       <c r="B32" t="s">
         <v>71</v>
       </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
       <c r="G32">
         <v>1</v>
       </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
       <c r="J32">
         <v>1</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
       </c>
       <c r="L32">
         <v>2</v>
@@ -2047,11 +3238,29 @@
       <c r="B33" t="s">
         <v>47</v>
       </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33">
         <v>1</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -2070,8 +3279,29 @@
       <c r="B34" t="s">
         <v>72</v>
       </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
       <c r="H34">
         <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
       </c>
       <c r="K34">
         <v>0</v>

</xml_diff>

<commit_message>
added GUI for input
</commit_message>
<xml_diff>
--- a/upper-level_writing_sample_output.xlsx
+++ b/upper-level_writing_sample_output.xlsx
@@ -708,24 +708,6 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
       <c r="L4">
         <v>3</v>
       </c>
@@ -749,24 +731,6 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
       <c r="L5">
         <v>3</v>
       </c>
@@ -784,28 +748,7 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
@@ -822,32 +765,11 @@
       <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
         <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -863,9 +785,6 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
       <c r="D8">
         <v>1</v>
       </c>
@@ -874,21 +793,6 @@
       </c>
       <c r="F8">
         <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -907,29 +811,8 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
       <c r="F9">
         <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
       </c>
       <c r="L9">
         <v>2</v>
@@ -945,32 +828,11 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -986,32 +848,11 @@
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
         <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
       </c>
       <c r="L11">
         <v>2</v>
@@ -1027,9 +868,6 @@
       <c r="B12" t="s">
         <v>51</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
       <c r="D12">
         <v>1</v>
       </c>
@@ -1037,21 +875,6 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
@@ -1071,29 +894,11 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
         <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -1109,32 +914,11 @@
       <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
       <c r="G14">
         <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
       </c>
       <c r="L14">
         <v>2</v>
@@ -1150,32 +934,11 @@
       <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
         <v>1</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1191,32 +954,14 @@
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
         <v>1</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
       </c>
       <c r="L16">
         <v>3</v>
@@ -1232,32 +977,11 @@
       <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
         <v>1</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
       </c>
       <c r="L17">
         <v>2</v>
@@ -1273,32 +997,11 @@
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
         <v>1</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
       </c>
       <c r="L18">
         <v>2</v>
@@ -1314,32 +1017,11 @@
       <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
         <v>1</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
       </c>
       <c r="L19">
         <v>2</v>
@@ -1355,32 +1037,11 @@
       <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
       <c r="J20">
         <v>1</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
       </c>
       <c r="L20">
         <v>2</v>
@@ -1396,32 +1057,11 @@
       <c r="B21" t="s">
         <v>35</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
       <c r="J21">
         <v>1</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
       </c>
       <c r="L21">
         <v>2</v>
@@ -1437,32 +1077,11 @@
       <c r="B22" t="s">
         <v>36</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
       <c r="J22">
         <v>1</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
       </c>
       <c r="L22">
         <v>2</v>
@@ -1478,32 +1097,11 @@
       <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23">
         <v>1</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -1519,32 +1117,8 @@
       <c r="B24" t="s">
         <v>38</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
       <c r="J24">
         <v>1</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -1560,32 +1134,11 @@
       <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
         <v>1</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
       </c>
       <c r="L25">
         <v>1</v>
@@ -1601,29 +1154,8 @@
       <c r="B26" t="s">
         <v>40</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
       <c r="I26">
         <v>1</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -1642,29 +1174,8 @@
       <c r="B27" t="s">
         <v>41</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
       <c r="G27">
         <v>1</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -1683,32 +1194,11 @@
       <c r="B28" t="s">
         <v>42</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
         <v>1</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
       </c>
       <c r="L28">
         <v>2</v>
@@ -1724,28 +1214,7 @@
       <c r="B29" t="s">
         <v>54</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
       <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
         <v>0</v>
       </c>
       <c r="K29">
@@ -1765,32 +1234,11 @@
       <c r="B30" t="s">
         <v>55</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
       <c r="J30">
         <v>1</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
       </c>
       <c r="L30">
         <v>1</v>
@@ -1806,29 +1254,8 @@
       <c r="B31" t="s">
         <v>45</v>
       </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
       <c r="H31">
         <v>1</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -1847,32 +1274,11 @@
       <c r="B32" t="s">
         <v>56</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
       <c r="G32">
         <v>0</v>
       </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
       <c r="J32">
         <v>1</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
       </c>
       <c r="L32">
         <v>1</v>
@@ -1888,29 +1294,11 @@
       <c r="B33" t="s">
         <v>57</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33">
         <v>1</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -1929,30 +1317,9 @@
       <c r="B34" t="s">
         <v>48</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
       <c r="H34">
         <v>1</v>
       </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
       <c r="K34">
         <v>1</v>
       </c>
@@ -1964,7 +1331,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C4:N28">
+  <conditionalFormatting sqref="C4:K35">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
@@ -2058,24 +1425,6 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
       <c r="L4">
         <v>2</v>
       </c>
@@ -2099,24 +1448,6 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
       <c r="L5">
         <v>3</v>
       </c>
@@ -2134,29 +1465,8 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
       <c r="F6">
         <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -2172,32 +1482,11 @@
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
         <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
       </c>
       <c r="L7">
         <v>2</v>
@@ -2213,9 +1502,6 @@
       <c r="B8" t="s">
         <v>60</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
       <c r="D8">
         <v>1</v>
       </c>
@@ -2223,21 +1509,6 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
@@ -2257,28 +1528,7 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
       <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
@@ -2295,32 +1545,11 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -2336,32 +1565,11 @@
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
         <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
       </c>
       <c r="L11">
         <v>2</v>
@@ -2377,9 +1585,6 @@
       <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
       <c r="D12">
         <v>1</v>
       </c>
@@ -2388,21 +1593,6 @@
       </c>
       <c r="F12">
         <v>1</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
       </c>
       <c r="L12">
         <v>3</v>
@@ -2421,29 +1611,11 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
         <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -2459,32 +1631,11 @@
       <c r="B14" t="s">
         <v>62</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
       <c r="G14">
         <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -2500,32 +1651,11 @@
       <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
         <v>1</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
       </c>
       <c r="L15">
         <v>2</v>
@@ -2541,32 +1671,14 @@
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
         <v>1</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
       </c>
       <c r="L16">
         <v>3</v>
@@ -2582,32 +1694,11 @@
       <c r="B17" t="s">
         <v>63</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
         <v>1</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -2623,32 +1714,11 @@
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
         <v>1</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
       </c>
       <c r="L18">
         <v>2</v>
@@ -2664,32 +1734,11 @@
       <c r="B19" t="s">
         <v>64</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
         <v>1</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
       </c>
       <c r="L19">
         <v>2</v>
@@ -2705,32 +1754,11 @@
       <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
       <c r="J20">
         <v>1</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
       </c>
       <c r="L20">
         <v>2</v>
@@ -2746,32 +1774,11 @@
       <c r="B21" t="s">
         <v>65</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
       <c r="H21">
         <v>0</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
       <c r="J21">
         <v>1</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -2787,32 +1794,11 @@
       <c r="B22" t="s">
         <v>66</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
       <c r="J22">
         <v>1</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
       </c>
       <c r="L22">
         <v>2</v>
@@ -2828,32 +1814,11 @@
       <c r="B23" t="s">
         <v>67</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23">
         <v>1</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -2869,32 +1834,8 @@
       <c r="B24" t="s">
         <v>38</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
       <c r="J24">
         <v>1</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -2910,32 +1851,11 @@
       <c r="B25" t="s">
         <v>39</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25">
         <v>1</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
       </c>
       <c r="L25">
         <v>2</v>
@@ -2951,29 +1871,8 @@
       <c r="B26" t="s">
         <v>40</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
       <c r="I26">
         <v>1</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -2992,29 +1891,8 @@
       <c r="B27" t="s">
         <v>68</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
       <c r="G27">
         <v>1</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -3033,31 +1911,10 @@
       <c r="B28" t="s">
         <v>69</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
@@ -3074,29 +1931,8 @@
       <c r="B29" t="s">
         <v>43</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
       <c r="I29">
         <v>1</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -3115,32 +1951,11 @@
       <c r="B30" t="s">
         <v>44</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
       <c r="H30">
         <v>1</v>
       </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
       <c r="J30">
         <v>1</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
       </c>
       <c r="L30">
         <v>2</v>
@@ -3156,28 +1971,7 @@
       <c r="B31" t="s">
         <v>70</v>
       </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
       <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
         <v>0</v>
       </c>
       <c r="K31">
@@ -3197,32 +1991,11 @@
       <c r="B32" t="s">
         <v>71</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
       <c r="J32">
         <v>1</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
       </c>
       <c r="L32">
         <v>2</v>
@@ -3238,29 +2011,11 @@
       <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33">
         <v>1</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -3279,30 +2034,9 @@
       <c r="B34" t="s">
         <v>72</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
       <c r="H34">
         <v>1</v>
       </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
       <c r="K34">
         <v>0</v>
       </c>
@@ -3314,7 +2048,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C4:N28">
+  <conditionalFormatting sqref="C4:K35">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>

</xml_diff>